<commit_message>
done for sample work
</commit_message>
<xml_diff>
--- a/src/test/resources/login_data.xlsx
+++ b/src/test/resources/login_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA\webdriver_java\excel_automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97667EE1-6A8F-41D1-BF04-A5DAB4C235D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DB5C37-68DD-4F48-8FEC-64F3B3248A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="3765" windowWidth="22050" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Details" sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>